<commit_message>
feat: add ML AEP calculator with independent daily probability draws
</commit_message>
<xml_diff>
--- a/results/cv_results/final_summary_table.xlsx
+++ b/results/cv_results/final_summary_table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="108">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -339,6 +339,18 @@
   </si>
   <si>
     <t xml:space="preserve">N. Ports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suyana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cierra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peru</t>
   </si>
 </sst>
 </file>
@@ -427,7 +439,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,13 +473,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFB66C"/>
-        <bgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFD428"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
         <bgColor rgb="FFB2B2B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD428"/>
+        <bgColor rgb="FFFFB66C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE16173"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,7 +543,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -572,7 +596,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,7 +604,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -612,11 +636,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -648,35 +672,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -684,35 +724,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -805,7 +849,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFE16173"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -827,7 +871,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF81D41A"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD428"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -2785,40 +2829,40 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="55.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="23" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="22.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="25.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="22.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="9.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="18.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="43" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="18.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="23" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="9.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="9.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="22.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="25.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="22.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="9.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="1" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="43" style="1" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="18.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4394,7 +4438,7 @@
         <v>0.120514281064367</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
@@ -4556,7 +4600,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD32"/>
+  <dimension ref="A1:XFD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
@@ -4567,7 +4611,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="10.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="14.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="14.53"/>
@@ -4635,8 +4679,8 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-      <c r="XFC1" s="0"/>
-      <c r="XFD1" s="0"/>
+      <c r="XFC1" s="1"/>
+      <c r="XFD1" s="1"/>
     </row>
     <row r="2" s="23" customFormat="true" ht="49.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
@@ -4714,7 +4758,7 @@
       <c r="Y2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="Z2" s="0"/>
+      <c r="Z2" s="1"/>
       <c r="XFC2" s="24"/>
       <c r="XFD2" s="24"/>
     </row>
@@ -4722,7 +4766,7 @@
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>124</v>
       </c>
       <c r="C3" s="3" t="n">
@@ -5605,15 +5649,15 @@
       <c r="B15" s="1" t="n">
         <v>658</v>
       </c>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0"/>
-      <c r="I17" s="0"/>
+      <c r="C17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
@@ -5742,7 +5786,7 @@
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="32" t="n">
+      <c r="B20" s="3" t="n">
         <f aca="false">5*658</f>
         <v>3290</v>
       </c>
@@ -5832,7 +5876,7 @@
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="32" t="n">
+      <c r="B21" s="3" t="n">
         <f aca="false">5*658</f>
         <v>3290</v>
       </c>
@@ -5922,7 +5966,7 @@
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="32" t="n">
+      <c r="B22" s="3" t="n">
         <f aca="false">6*658</f>
         <v>3948</v>
       </c>
@@ -6092,7 +6136,7 @@
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="32" t="n">
+      <c r="B24" s="3" t="n">
         <f aca="false">7*658</f>
         <v>4606</v>
       </c>
@@ -6680,9 +6724,6 @@
       <c r="Y30" s="31" t="n">
         <v>0.52832456799399</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:Y12"/>
@@ -6702,10 +6743,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6839,482 +6880,482 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="32" t="n">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="32" t="n">
+      <c r="C3" s="3" t="n">
         <v>3290</v>
       </c>
-      <c r="D3" s="32" t="n">
+      <c r="D3" s="3" t="n">
         <v>424364.845714286</v>
       </c>
-      <c r="E3" s="32" t="n">
+      <c r="E3" s="3" t="n">
         <v>410566.530612245</v>
       </c>
-      <c r="F3" s="32" t="n">
+      <c r="F3" s="3" t="n">
         <v>572525.714285715</v>
       </c>
-      <c r="G3" s="32" t="n">
+      <c r="G3" s="3" t="n">
         <v>74.86275</v>
       </c>
-      <c r="H3" s="32" t="n">
+      <c r="H3" s="3" t="n">
         <v>72.4285714285714</v>
       </c>
-      <c r="I3" s="32" t="n">
+      <c r="I3" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="J3" s="33" t="n">
+      <c r="J3" s="25" t="n">
         <v>303132.525714286</v>
       </c>
-      <c r="K3" s="33" t="n">
+      <c r="K3" s="25" t="n">
         <v>430868.114285713</v>
       </c>
-      <c r="L3" s="34" t="n">
+      <c r="L3" s="26" t="n">
         <v>121232.32</v>
       </c>
-      <c r="M3" s="34" t="n">
+      <c r="M3" s="26" t="n">
         <v>181394.285714286</v>
       </c>
-      <c r="N3" s="35" t="n">
+      <c r="N3" s="33" t="n">
         <v>106744.868571429</v>
       </c>
-      <c r="O3" s="35" t="n">
+      <c r="O3" s="33" t="n">
         <v>181394.285714286</v>
       </c>
-      <c r="P3" s="36" t="n">
+      <c r="P3" s="28" t="n">
         <v>0.73956878310537</v>
       </c>
-      <c r="Q3" s="36" t="n">
+      <c r="Q3" s="28" t="n">
         <v>0.26043121689463</v>
       </c>
-      <c r="R3" s="37" t="n">
+      <c r="R3" s="34" t="n">
         <v>1.13572035473422</v>
       </c>
-      <c r="S3" s="38" t="n">
+      <c r="S3" s="35" t="n">
         <v>375</v>
       </c>
-      <c r="T3" s="38" t="n">
+      <c r="T3" s="35" t="n">
         <v>150</v>
       </c>
-      <c r="U3" s="38" t="n">
+      <c r="U3" s="35" t="n">
         <v>1904</v>
       </c>
-      <c r="V3" s="38" t="n">
+      <c r="V3" s="35" t="n">
         <v>132</v>
       </c>
-      <c r="W3" s="39" t="n">
+      <c r="W3" s="36" t="n">
         <v>0.714285714285714</v>
       </c>
-      <c r="X3" s="39" t="n">
+      <c r="X3" s="36" t="n">
         <v>0.739644970414201</v>
       </c>
-      <c r="Y3" s="39" t="n">
+      <c r="Y3" s="36" t="n">
         <v>0.88988676298321</v>
       </c>
-      <c r="Z3" s="39" t="n">
+      <c r="Z3" s="36" t="n">
         <v>0.726744186046512</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="32" t="n">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="32" t="n">
+      <c r="C4" s="3" t="n">
         <v>3290</v>
       </c>
-      <c r="D4" s="32" t="n">
+      <c r="D4" s="3" t="n">
         <v>4786279.85852381</v>
       </c>
-      <c r="E4" s="32" t="n">
+      <c r="E4" s="3" t="n">
         <v>4658959.23809524</v>
       </c>
-      <c r="F4" s="32" t="n">
+      <c r="F4" s="3" t="n">
         <v>6406068.95238095</v>
       </c>
-      <c r="G4" s="32" t="n">
+      <c r="G4" s="3" t="n">
         <v>82.18625</v>
       </c>
-      <c r="H4" s="32" t="n">
+      <c r="H4" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="I4" s="32" t="n">
+      <c r="I4" s="3" t="n">
         <v>110</v>
       </c>
-      <c r="J4" s="33" t="n">
+      <c r="J4" s="25" t="n">
         <v>3198288.16146667</v>
       </c>
-      <c r="K4" s="33" t="n">
+      <c r="K4" s="25" t="n">
         <v>4600722.24761905</v>
       </c>
-      <c r="L4" s="34" t="n">
+      <c r="L4" s="26" t="n">
         <v>1587991.69705715</v>
       </c>
-      <c r="M4" s="34" t="n">
+      <c r="M4" s="26" t="n">
         <v>2445953.6</v>
       </c>
-      <c r="N4" s="35" t="n">
+      <c r="N4" s="33" t="n">
         <v>1428698.96885715</v>
       </c>
-      <c r="O4" s="35" t="n">
+      <c r="O4" s="33" t="n">
         <v>2329479.61904762</v>
       </c>
-      <c r="P4" s="36" t="n">
+      <c r="P4" s="28" t="n">
         <v>0.691224780053114</v>
       </c>
-      <c r="Q4" s="36" t="n">
+      <c r="Q4" s="28" t="n">
         <v>0.308775219946886</v>
       </c>
-      <c r="R4" s="37" t="n">
+      <c r="R4" s="34" t="n">
         <v>1.11149495567105</v>
       </c>
-      <c r="S4" s="38" t="n">
+      <c r="S4" s="35" t="n">
         <v>386</v>
       </c>
-      <c r="T4" s="38" t="n">
+      <c r="T4" s="35" t="n">
         <v>191</v>
       </c>
-      <c r="U4" s="38" t="n">
+      <c r="U4" s="35" t="n">
         <v>1813</v>
       </c>
-      <c r="V4" s="38" t="n">
+      <c r="V4" s="35" t="n">
         <v>174</v>
       </c>
-      <c r="W4" s="39" t="n">
+      <c r="W4" s="36" t="n">
         <v>0.668977469670711</v>
       </c>
-      <c r="X4" s="39" t="n">
+      <c r="X4" s="36" t="n">
         <v>0.689285714285714</v>
       </c>
-      <c r="Y4" s="39" t="n">
+      <c r="Y4" s="36" t="n">
         <v>0.857644305772231</v>
       </c>
-      <c r="Z4" s="39" t="n">
+      <c r="Z4" s="36" t="n">
         <v>0.678979771328056</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="32" t="n">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="n">
+      <c r="C5" s="3" t="n">
         <v>3948</v>
       </c>
-      <c r="D5" s="32" t="n">
+      <c r="D5" s="3" t="n">
         <v>1225923.70564286</v>
       </c>
-      <c r="E5" s="32" t="n">
+      <c r="E5" s="3" t="n">
         <v>1243428.97959184</v>
       </c>
-      <c r="F5" s="32" t="n">
+      <c r="F5" s="3" t="n">
         <v>1614592.53</v>
       </c>
-      <c r="G5" s="32" t="n">
+      <c r="G5" s="3" t="n">
         <v>87.3245</v>
       </c>
-      <c r="H5" s="32" t="n">
+      <c r="H5" s="3" t="n">
         <v>88.5714285714286</v>
       </c>
-      <c r="I5" s="32" t="n">
+      <c r="I5" s="3" t="n">
         <v>115.01</v>
       </c>
-      <c r="J5" s="33" t="n">
+      <c r="J5" s="25" t="n">
         <v>764797.567178574</v>
       </c>
-      <c r="K5" s="33" t="n">
+      <c r="K5" s="25" t="n">
         <v>1080981</v>
       </c>
-      <c r="L5" s="34" t="n">
+      <c r="L5" s="26" t="n">
         <v>461126.138464286</v>
       </c>
-      <c r="M5" s="34" t="n">
+      <c r="M5" s="26" t="n">
         <v>701935.714285716</v>
       </c>
-      <c r="N5" s="35" t="n">
+      <c r="N5" s="33" t="n">
         <v>470900.593285714</v>
       </c>
-      <c r="O5" s="35" t="n">
+      <c r="O5" s="33" t="n">
         <v>715974.428571426</v>
       </c>
-      <c r="P5" s="36" t="n">
+      <c r="P5" s="28" t="n">
         <v>0.618919402527246</v>
       </c>
-      <c r="Q5" s="36" t="n">
+      <c r="Q5" s="28" t="n">
         <v>0.381080597472754</v>
       </c>
-      <c r="R5" s="37" t="n">
+      <c r="R5" s="34" t="n">
         <v>0.979243061145396</v>
       </c>
-      <c r="S5" s="38" t="n">
+      <c r="S5" s="35" t="n">
         <v>382</v>
       </c>
-      <c r="T5" s="38" t="n">
+      <c r="T5" s="35" t="n">
         <v>230</v>
       </c>
-      <c r="U5" s="38" t="n">
+      <c r="U5" s="35" t="n">
         <v>1707</v>
       </c>
-      <c r="V5" s="38" t="n">
+      <c r="V5" s="35" t="n">
         <v>238</v>
       </c>
-      <c r="W5" s="39" t="n">
+      <c r="W5" s="36" t="n">
         <v>0.624183006535948</v>
       </c>
-      <c r="X5" s="39" t="n">
+      <c r="X5" s="36" t="n">
         <v>0.616129032258065</v>
       </c>
-      <c r="Y5" s="39" t="n">
+      <c r="Y5" s="36" t="n">
         <v>0.816973015252249</v>
       </c>
-      <c r="Z5" s="39" t="n">
+      <c r="Z5" s="36" t="n">
         <v>0.62012987012987</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="32" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="32" t="n">
+      <c r="C6" s="3" t="n">
         <v>5236</v>
       </c>
-      <c r="D6" s="32" t="n">
+      <c r="D6" s="3" t="n">
         <v>3754155.9</v>
       </c>
-      <c r="E6" s="32" t="n">
+      <c r="E6" s="3" t="n">
         <v>4103314.28571429</v>
       </c>
-      <c r="F6" s="32" t="n">
+      <c r="F6" s="3" t="n">
         <v>5385600</v>
       </c>
-      <c r="G6" s="32" t="n">
+      <c r="G6" s="3" t="n">
         <v>50.18925</v>
       </c>
-      <c r="H6" s="32" t="n">
+      <c r="H6" s="3" t="n">
         <v>54.8571428571429</v>
       </c>
-      <c r="I6" s="32" t="n">
+      <c r="I6" s="3" t="n">
         <v>72</v>
       </c>
-      <c r="J6" s="33" t="n">
+      <c r="J6" s="25" t="n">
         <v>2113343.1</v>
       </c>
-      <c r="K6" s="33" t="n">
+      <c r="K6" s="25" t="n">
         <v>3515600</v>
       </c>
-      <c r="L6" s="34" t="n">
+      <c r="L6" s="26" t="n">
         <v>1640812.8</v>
       </c>
-      <c r="M6" s="34" t="n">
+      <c r="M6" s="26" t="n">
         <v>2842400</v>
       </c>
-      <c r="N6" s="35" t="n">
+      <c r="N6" s="33" t="n">
         <v>1992915.1</v>
       </c>
-      <c r="O6" s="35" t="n">
+      <c r="O6" s="33" t="n">
         <v>3291200</v>
       </c>
-      <c r="P6" s="36" t="n">
+      <c r="P6" s="28" t="n">
         <v>0.514663958540162</v>
       </c>
-      <c r="Q6" s="36" t="n">
+      <c r="Q6" s="28" t="n">
         <v>0.485336041459838</v>
       </c>
-      <c r="R6" s="37" t="n">
+      <c r="R6" s="34" t="n">
         <v>0.823322980492245</v>
       </c>
-      <c r="S6" s="38" t="n">
+      <c r="S6" s="35" t="n">
         <v>198</v>
       </c>
-      <c r="T6" s="38" t="n">
+      <c r="T6" s="35" t="n">
         <v>155</v>
       </c>
-      <c r="U6" s="38" t="n">
+      <c r="U6" s="35" t="n">
         <v>2018</v>
       </c>
-      <c r="V6" s="38" t="n">
+      <c r="V6" s="35" t="n">
         <v>186</v>
       </c>
-      <c r="W6" s="39" t="n">
+      <c r="W6" s="36" t="n">
         <v>0.560906515580737</v>
       </c>
-      <c r="X6" s="39" t="n">
+      <c r="X6" s="36" t="n">
         <v>0.515625</v>
       </c>
-      <c r="Y6" s="39" t="n">
+      <c r="Y6" s="36" t="n">
         <v>0.866640594446617</v>
       </c>
-      <c r="Z6" s="39" t="n">
+      <c r="Z6" s="36" t="n">
         <v>0.537313432835821</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="32" t="n">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C7" s="32" t="n">
+      <c r="C7" s="3" t="n">
         <v>4606</v>
       </c>
-      <c r="D7" s="32" t="n">
+      <c r="D7" s="3" t="n">
         <v>894366.179999999</v>
       </c>
-      <c r="E7" s="32" t="n">
+      <c r="E7" s="3" t="n">
         <v>922855.714285715</v>
       </c>
-      <c r="F7" s="32" t="n">
+      <c r="F7" s="3" t="n">
         <v>1295700</v>
       </c>
-      <c r="G7" s="32" t="n">
+      <c r="G7" s="3" t="n">
         <v>48.318</v>
       </c>
-      <c r="H7" s="32" t="n">
+      <c r="H7" s="3" t="n">
         <v>49.8571428571429</v>
       </c>
-      <c r="I7" s="32" t="n">
+      <c r="I7" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="J7" s="33" t="n">
+      <c r="J7" s="25" t="n">
         <v>460681.5075</v>
       </c>
-      <c r="K7" s="33" t="n">
+      <c r="K7" s="25" t="n">
         <v>795930.000000002</v>
       </c>
-      <c r="L7" s="34" t="n">
+      <c r="L7" s="26" t="n">
         <v>433684.6725</v>
       </c>
-      <c r="M7" s="34" t="n">
+      <c r="M7" s="26" t="n">
         <v>703379.999999999</v>
       </c>
-      <c r="N7" s="35" t="n">
+      <c r="N7" s="33" t="n">
         <v>455693.0625</v>
       </c>
-      <c r="O7" s="35" t="n">
+      <c r="O7" s="33" t="n">
         <v>758909.999999998</v>
       </c>
-      <c r="P7" s="36" t="n">
+      <c r="P7" s="28" t="n">
         <v>0.502721837315935</v>
       </c>
-      <c r="Q7" s="36" t="n">
+      <c r="Q7" s="28" t="n">
         <v>0.497278162684065</v>
       </c>
-      <c r="R7" s="37" t="n">
+      <c r="R7" s="34" t="n">
         <v>0.951703478040112</v>
       </c>
-      <c r="S7" s="38" t="n">
+      <c r="S7" s="35" t="n">
         <v>174</v>
       </c>
-      <c r="T7" s="38" t="n">
+      <c r="T7" s="35" t="n">
         <v>164</v>
       </c>
-      <c r="U7" s="38" t="n">
+      <c r="U7" s="35" t="n">
         <v>2044</v>
       </c>
-      <c r="V7" s="38" t="n">
+      <c r="V7" s="35" t="n">
         <v>175</v>
       </c>
-      <c r="W7" s="39" t="n">
+      <c r="W7" s="36" t="n">
         <v>0.514792899408284</v>
       </c>
-      <c r="X7" s="39" t="n">
+      <c r="X7" s="36" t="n">
         <v>0.498567335243553</v>
       </c>
-      <c r="Y7" s="39" t="n">
+      <c r="Y7" s="36" t="n">
         <v>0.867422761048103</v>
       </c>
-      <c r="Z7" s="39" t="n">
+      <c r="Z7" s="36" t="n">
         <v>0.506550218340611</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="32" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C8" s="32" t="n">
+      <c r="C8" s="3" t="n">
         <v>3853</v>
       </c>
-      <c r="D8" s="32" t="n">
+      <c r="D8" s="3" t="n">
         <v>987757.35581044</v>
       </c>
-      <c r="E8" s="32" t="n">
+      <c r="E8" s="3" t="n">
         <v>949525.577708006</v>
       </c>
-      <c r="F8" s="32" t="n">
+      <c r="F8" s="3" t="n">
         <v>1560253.2967033</v>
       </c>
-      <c r="G8" s="32" t="n">
+      <c r="G8" s="3" t="n">
         <v>31.65375</v>
       </c>
-      <c r="H8" s="32" t="n">
+      <c r="H8" s="3" t="n">
         <v>30.4285714285714</v>
       </c>
-      <c r="I8" s="32" t="n">
+      <c r="I8" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="J8" s="33" t="n">
+      <c r="J8" s="25" t="n">
         <v>440638.934788462</v>
       </c>
-      <c r="K8" s="33" t="n">
+      <c r="K8" s="25" t="n">
         <v>873741.846153846</v>
       </c>
-      <c r="L8" s="34" t="n">
+      <c r="L8" s="26" t="n">
         <v>547118.421021978</v>
       </c>
-      <c r="M8" s="34" t="n">
+      <c r="M8" s="26" t="n">
         <v>967357.043956044</v>
       </c>
-      <c r="N8" s="35" t="n">
+      <c r="N8" s="33" t="n">
         <v>495037.165978022</v>
       </c>
-      <c r="O8" s="35" t="n">
+      <c r="O8" s="33" t="n">
         <v>936151.978021978</v>
       </c>
-      <c r="P8" s="36" t="n">
+      <c r="P8" s="28" t="n">
         <v>0.470931056620449</v>
       </c>
-      <c r="Q8" s="36" t="n">
+      <c r="Q8" s="28" t="n">
         <v>0.529068943379551</v>
       </c>
-      <c r="R8" s="37" t="n">
+      <c r="R8" s="34" t="n">
         <v>1.10520675743823</v>
       </c>
-      <c r="S8" s="38" t="n">
+      <c r="S8" s="35" t="n">
         <v>100</v>
       </c>
-      <c r="T8" s="38" t="n">
+      <c r="T8" s="35" t="n">
         <v>122</v>
       </c>
-      <c r="U8" s="38" t="n">
+      <c r="U8" s="35" t="n">
         <v>2222</v>
       </c>
-      <c r="V8" s="38" t="n">
+      <c r="V8" s="35" t="n">
         <v>113</v>
       </c>
-      <c r="W8" s="39" t="n">
+      <c r="W8" s="36" t="n">
         <v>0.450450450450451</v>
       </c>
-      <c r="X8" s="39" t="n">
+      <c r="X8" s="36" t="n">
         <v>0.469483568075117</v>
       </c>
-      <c r="Y8" s="39" t="n">
+      <c r="Y8" s="36" t="n">
         <v>0.908095424325381</v>
       </c>
-      <c r="Z8" s="39" t="n">
+      <c r="Z8" s="36" t="n">
         <v>0.459770114942529</v>
       </c>
     </row>
@@ -7325,76 +7366,76 @@
       <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="32" t="n">
+      <c r="C9" s="3" t="n">
         <v>3948</v>
       </c>
-      <c r="D9" s="32" t="n">
+      <c r="D9" s="3" t="n">
         <v>1332003.92</v>
       </c>
-      <c r="E9" s="32" t="n">
+      <c r="E9" s="3" t="n">
         <v>318794.285714286</v>
       </c>
-      <c r="F9" s="32" t="n">
+      <c r="F9" s="3" t="n">
         <v>2279040</v>
       </c>
-      <c r="G9" s="32" t="n">
+      <c r="G9" s="3" t="n">
         <v>28.054</v>
       </c>
-      <c r="H9" s="32" t="n">
+      <c r="H9" s="3" t="n">
         <v>6.71428571428571</v>
       </c>
-      <c r="I9" s="32" t="n">
+      <c r="I9" s="3" t="n">
         <v>48</v>
       </c>
-      <c r="J9" s="33" t="n">
+      <c r="J9" s="25" t="n">
         <v>199594.05</v>
       </c>
-      <c r="K9" s="33" t="n">
+      <c r="K9" s="25" t="n">
         <v>569760</v>
       </c>
-      <c r="L9" s="34" t="n">
+      <c r="L9" s="26" t="n">
         <v>1132409.87</v>
       </c>
-      <c r="M9" s="34" t="n">
+      <c r="M9" s="26" t="n">
         <v>1946680</v>
       </c>
-      <c r="N9" s="35" t="n">
+      <c r="N9" s="33" t="n">
         <v>88490.85</v>
       </c>
-      <c r="O9" s="35" t="n">
+      <c r="O9" s="33" t="n">
         <v>332360</v>
       </c>
-      <c r="P9" s="36" t="n">
+      <c r="P9" s="28" t="n">
         <v>0.69283065512979</v>
       </c>
-      <c r="Q9" s="36" t="n">
+      <c r="Q9" s="28" t="n">
         <v>0.30716934487021</v>
       </c>
-      <c r="R9" s="37" t="n">
+      <c r="R9" s="34" t="n">
         <v>12.7969148222669</v>
       </c>
-      <c r="S9" s="38" t="n">
+      <c r="S9" s="35" t="n">
         <v>34</v>
       </c>
-      <c r="T9" s="38" t="n">
+      <c r="T9" s="35" t="n">
         <v>167</v>
       </c>
-      <c r="U9" s="38" t="n">
+      <c r="U9" s="35" t="n">
         <v>2343</v>
       </c>
-      <c r="V9" s="38" t="n">
+      <c r="V9" s="35" t="n">
         <v>13</v>
       </c>
-      <c r="W9" s="39" t="n">
+      <c r="W9" s="37" t="n">
         <v>0.169154228855721</v>
       </c>
-      <c r="X9" s="39" t="n">
+      <c r="X9" s="37" t="n">
         <v>0.723404255319149</v>
       </c>
-      <c r="Y9" s="39" t="n">
+      <c r="Y9" s="37" t="n">
         <v>0.92960500586625</v>
       </c>
-      <c r="Z9" s="39" t="n">
+      <c r="Z9" s="37" t="n">
         <v>0.274193548387097</v>
       </c>
     </row>
@@ -7405,156 +7446,156 @@
       <c r="B10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="32" t="n">
+      <c r="C10" s="3" t="n">
         <v>2827</v>
       </c>
-      <c r="D10" s="32" t="n">
+      <c r="D10" s="3" t="n">
         <v>1205510.23960714</v>
       </c>
-      <c r="E10" s="32" t="n">
+      <c r="E10" s="3" t="n">
         <v>1218148.53061225</v>
       </c>
-      <c r="F10" s="32" t="n">
+      <c r="F10" s="3" t="n">
         <v>1800152.82857143</v>
       </c>
-      <c r="G10" s="32" t="n">
+      <c r="G10" s="3" t="n">
         <v>38.17125</v>
       </c>
-      <c r="H10" s="32" t="n">
+      <c r="H10" s="3" t="n">
         <v>38.5714285714286</v>
       </c>
-      <c r="I10" s="32" t="n">
+      <c r="I10" s="3" t="n">
         <v>57</v>
       </c>
-      <c r="J10" s="33" t="n">
+      <c r="J10" s="25" t="n">
         <v>313131.847285714</v>
       </c>
-      <c r="K10" s="33" t="n">
+      <c r="K10" s="25" t="n">
         <v>663214.2</v>
       </c>
-      <c r="L10" s="34" t="n">
+      <c r="L10" s="26" t="n">
         <v>892378.392321429</v>
       </c>
-      <c r="M10" s="34" t="n">
+      <c r="M10" s="26" t="n">
         <v>1421489.10199999</v>
       </c>
-      <c r="N10" s="35" t="n">
+      <c r="N10" s="33" t="n">
         <v>890499.285421429</v>
       </c>
-      <c r="O10" s="35" t="n">
+      <c r="O10" s="33" t="n">
         <v>1579081.42857143</v>
       </c>
-      <c r="P10" s="36" t="n">
+      <c r="P10" s="28" t="n">
         <v>0.260155988638674</v>
       </c>
-      <c r="Q10" s="36" t="n">
+      <c r="Q10" s="28" t="n">
         <v>0.739844011361326</v>
       </c>
-      <c r="R10" s="37" t="n">
+      <c r="R10" s="34" t="n">
         <v>1.00211017227163</v>
       </c>
-      <c r="S10" s="38" t="n">
+      <c r="S10" s="35" t="n">
         <v>69</v>
       </c>
-      <c r="T10" s="38" t="n">
+      <c r="T10" s="35" t="n">
         <v>199</v>
       </c>
-      <c r="U10" s="38" t="n">
+      <c r="U10" s="35" t="n">
         <v>2095</v>
       </c>
-      <c r="V10" s="38" t="n">
+      <c r="V10" s="35" t="n">
         <v>201</v>
       </c>
-      <c r="W10" s="39" t="n">
+      <c r="W10" s="37" t="n">
         <v>0.257462686567164</v>
       </c>
-      <c r="X10" s="39" t="n">
+      <c r="X10" s="37" t="n">
         <v>0.255555555555556</v>
       </c>
-      <c r="Y10" s="39" t="n">
+      <c r="Y10" s="37" t="n">
         <v>0.84399375975039</v>
       </c>
-      <c r="Z10" s="39" t="n">
+      <c r="Z10" s="37" t="n">
         <v>0.256505576208178</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="38" t="n">
         <v>14</v>
       </c>
-      <c r="C11" s="32" t="n">
+      <c r="C11" s="39" t="n">
         <v>14424</v>
       </c>
-      <c r="D11" s="32" t="n">
+      <c r="D11" s="39" t="n">
         <v>4267619.12172245</v>
       </c>
-      <c r="E11" s="32" t="n">
+      <c r="E11" s="40" t="n">
         <v>1346839.94868805</v>
       </c>
-      <c r="F11" s="32" t="n">
+      <c r="F11" s="40" t="n">
         <v>6989634.90612245</v>
       </c>
-      <c r="G11" s="32" t="n">
+      <c r="G11" s="40" t="n">
         <v>26.25425</v>
       </c>
-      <c r="H11" s="32" t="n">
+      <c r="H11" s="40" t="n">
         <v>8.28571428571429</v>
       </c>
-      <c r="I11" s="32" t="n">
+      <c r="I11" s="40" t="n">
         <v>43</v>
       </c>
-      <c r="J11" s="33" t="n">
+      <c r="J11" s="40" t="n">
         <v>597654.421885714</v>
       </c>
-      <c r="K11" s="33" t="n">
+      <c r="K11" s="40" t="n">
         <v>1788046.13877551</v>
       </c>
-      <c r="L11" s="34" t="n">
+      <c r="L11" s="40" t="n">
         <v>3669964.69983673</v>
       </c>
-      <c r="M11" s="34" t="n">
+      <c r="M11" s="40" t="n">
         <v>6176886.66122449</v>
       </c>
-      <c r="N11" s="35" t="n">
+      <c r="N11" s="41" t="n">
         <v>642558.762416327</v>
       </c>
-      <c r="O11" s="35" t="n">
+      <c r="O11" s="41" t="n">
         <v>1788046.13877551</v>
       </c>
-      <c r="P11" s="36" t="n">
+      <c r="P11" s="42" t="n">
         <v>0.481896523477178</v>
       </c>
-      <c r="Q11" s="36" t="n">
+      <c r="Q11" s="42" t="n">
         <v>0.518103476522822</v>
       </c>
       <c r="R11" s="37" t="n">
         <v>5.71148494814064</v>
       </c>
-      <c r="S11" s="38" t="n">
+      <c r="S11" s="43" t="n">
         <v>28</v>
       </c>
-      <c r="T11" s="38" t="n">
+      <c r="T11" s="43" t="n">
         <v>158</v>
       </c>
-      <c r="U11" s="38" t="n">
+      <c r="U11" s="43" t="n">
         <v>2341</v>
       </c>
-      <c r="V11" s="38" t="n">
+      <c r="V11" s="43" t="n">
         <v>30</v>
       </c>
-      <c r="W11" s="39" t="n">
+      <c r="W11" s="37" t="n">
         <v>0.150537634408602</v>
       </c>
-      <c r="X11" s="39" t="n">
+      <c r="X11" s="37" t="n">
         <v>0.482758620689655</v>
       </c>
-      <c r="Y11" s="39" t="n">
+      <c r="Y11" s="37" t="n">
         <v>0.926476339460305</v>
       </c>
-      <c r="Z11" s="39" t="n">
+      <c r="Z11" s="37" t="n">
         <v>0.229508196721312</v>
       </c>
     </row>
@@ -7565,158 +7606,213 @@
       <c r="B12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="32" t="n">
+      <c r="C12" s="3" t="n">
         <v>2109</v>
       </c>
-      <c r="D12" s="32" t="n">
+      <c r="D12" s="3" t="n">
         <v>1042988.59594286</v>
       </c>
-      <c r="E12" s="32" t="n">
+      <c r="E12" s="3" t="n">
         <v>175740.817959184</v>
       </c>
-      <c r="F12" s="32" t="n">
+      <c r="F12" s="3" t="n">
         <v>1926517.26857143</v>
       </c>
-      <c r="G12" s="32" t="n">
+      <c r="G12" s="3" t="n">
         <v>44.935</v>
       </c>
-      <c r="H12" s="32" t="n">
+      <c r="H12" s="3" t="n">
         <v>7.57142857142857</v>
       </c>
-      <c r="I12" s="32" t="n">
+      <c r="I12" s="3" t="n">
         <v>83</v>
       </c>
-      <c r="J12" s="33" t="n">
+      <c r="J12" s="25" t="n">
         <v>40758.6063085714</v>
       </c>
-      <c r="K12" s="33" t="n">
+      <c r="K12" s="25" t="n">
         <v>208899.462857143</v>
       </c>
-      <c r="L12" s="34" t="n">
+      <c r="L12" s="26" t="n">
         <v>1002229.98963429</v>
       </c>
-      <c r="M12" s="34" t="n">
+      <c r="M12" s="26" t="n">
         <v>1856884.11428571</v>
       </c>
-      <c r="N12" s="35" t="n">
+      <c r="N12" s="33" t="n">
         <v>124683.965511429</v>
       </c>
-      <c r="O12" s="35" t="n">
+      <c r="O12" s="33" t="n">
         <v>371376.822857143</v>
       </c>
-      <c r="P12" s="36" t="n">
+      <c r="P12" s="28" t="n">
         <v>0.246361053628423</v>
       </c>
-      <c r="Q12" s="36" t="n">
+      <c r="Q12" s="28" t="n">
         <v>0.753638946371577</v>
       </c>
-      <c r="R12" s="37" t="n">
+      <c r="R12" s="34" t="n">
         <v>8.03816260995021</v>
       </c>
-      <c r="S12" s="38" t="n">
+      <c r="S12" s="35" t="n">
         <v>12</v>
       </c>
-      <c r="T12" s="38" t="n">
+      <c r="T12" s="35" t="n">
         <v>300</v>
       </c>
-      <c r="U12" s="38" t="n">
+      <c r="U12" s="35" t="n">
         <v>2198</v>
       </c>
-      <c r="V12" s="38" t="n">
+      <c r="V12" s="35" t="n">
         <v>41</v>
       </c>
-      <c r="W12" s="39" t="n">
+      <c r="W12" s="37" t="n">
         <v>0.0384615384615385</v>
       </c>
-      <c r="X12" s="39" t="n">
+      <c r="X12" s="37" t="n">
         <v>0.226415094339623</v>
       </c>
-      <c r="Y12" s="39" t="n">
+      <c r="Y12" s="37" t="n">
         <v>0.866326930615445</v>
       </c>
-      <c r="Z12" s="39" t="n">
+      <c r="Z12" s="37" t="n">
         <v>0.0657534246575343</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="40" t="n">
+      <c r="B13" s="44" t="n">
         <f aca="false">SUM(B3:B12)</f>
         <v>69</v>
       </c>
-      <c r="C13" s="41" t="n">
+      <c r="C13" s="45" t="n">
         <v>47531</v>
       </c>
-      <c r="D13" s="41" t="n">
+      <c r="D13" s="45" t="n">
         <v>19920969.7229638</v>
       </c>
-      <c r="E13" s="41" t="n">
+      <c r="E13" s="45" t="n">
         <v>15348173.9089811</v>
       </c>
-      <c r="F13" s="41" t="n">
+      <c r="F13" s="45" t="n">
         <v>29830085.4966353</v>
       </c>
-      <c r="G13" s="41" t="n">
+      <c r="G13" s="45" t="n">
         <v>511.949</v>
       </c>
-      <c r="H13" s="41" t="n">
+      <c r="H13" s="45" t="n">
         <v>437.285714285714</v>
       </c>
-      <c r="I13" s="41" t="n">
+      <c r="I13" s="45" t="n">
         <v>749.01</v>
       </c>
-      <c r="J13" s="42" t="n">
+      <c r="J13" s="46" t="n">
         <v>8432020.72212799</v>
       </c>
-      <c r="K13" s="42" t="n">
+      <c r="K13" s="46" t="n">
         <v>14527763.0096913</v>
       </c>
-      <c r="L13" s="43" t="n">
+      <c r="L13" s="47" t="n">
         <v>11488949.0008359</v>
       </c>
-      <c r="M13" s="43" t="n">
+      <c r="M13" s="47" t="n">
         <v>19244360.5214662</v>
       </c>
-      <c r="N13" s="44" t="n">
+      <c r="N13" s="48" t="n">
         <v>6696222.6225415</v>
       </c>
-      <c r="O13" s="44" t="n">
+      <c r="O13" s="48" t="n">
         <v>12283974.7015594</v>
       </c>
-      <c r="P13" s="45" t="n">
+      <c r="P13" s="49" t="n">
         <v>0.557369453281505</v>
       </c>
-      <c r="Q13" s="45" t="n">
+      <c r="Q13" s="49" t="n">
         <v>0.442630546718495</v>
       </c>
-      <c r="R13" s="46" t="n">
+      <c r="R13" s="50" t="n">
         <v>1.71573581830458</v>
       </c>
-      <c r="S13" s="47" t="n">
+      <c r="S13" s="51" t="n">
         <v>1758</v>
       </c>
-      <c r="T13" s="47" t="n">
+      <c r="T13" s="51" t="n">
         <v>1836</v>
       </c>
-      <c r="U13" s="47" t="n">
+      <c r="U13" s="51" t="n">
         <v>20685</v>
       </c>
-      <c r="V13" s="47" t="n">
+      <c r="V13" s="51" t="n">
         <v>1303</v>
       </c>
-      <c r="W13" s="48" t="n">
+      <c r="W13" s="52" t="n">
         <v>0.489148580968281</v>
       </c>
-      <c r="X13" s="48" t="n">
+      <c r="X13" s="52" t="n">
         <v>0.574322116955243</v>
       </c>
-      <c r="Y13" s="48" t="n">
+      <c r="Y13" s="52" t="n">
         <v>0.877296536627316</v>
       </c>
-      <c r="Z13" s="48" t="n">
+      <c r="Z13" s="52" t="n">
         <v>0.52832456799399</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="26" t="n">
+        <f aca="false">L3</f>
+        <v>121232.32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="53" t="n">
+        <f aca="false">N3</f>
+        <v>106744.868571429</v>
+      </c>
+      <c r="L18" s="25" t="n">
+        <f aca="false">J3</f>
+        <v>303132.525714286</v>
+      </c>
+      <c r="M18" s="3" t="n">
+        <f aca="false">L18+K18</f>
+        <v>409877.394285715</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <f aca="false">D3</f>
+        <v>424364.845714286</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L19" s="3" t="n">
+        <f aca="false">L18+L17</f>
+        <v>424364.845714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added event level detection script
</commit_message>
<xml_diff>
--- a/results/cv_results/final_summary_table.xlsx
+++ b/results/cv_results/final_summary_table.xlsx
@@ -549,7 +549,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -764,10 +764,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1098,7 +1094,7 @@
   <dimension ref="A1:AU12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="J13 L13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2841,7 +2837,7 @@
   <dimension ref="A1:AU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+      <selection pane="topLeft" activeCell="Z1" activeCellId="2" sqref="J13 L13 Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4621,7 +4617,7 @@
   <dimension ref="A1:AU12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="J13 L13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6364,7 +6360,7 @@
   <dimension ref="A1:AU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="2" sqref="J13 L13 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8144,7 +8140,7 @@
   <dimension ref="A1:XFD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="2" sqref="J13 L13 C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8220,8 +8216,8 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-      <c r="XFC1" s="0"/>
-      <c r="XFD1" s="0"/>
+      <c r="XFC1" s="1"/>
+      <c r="XFD1" s="1"/>
     </row>
     <row r="2" s="23" customFormat="true" ht="48.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
@@ -8300,8 +8296,8 @@
         <v>101</v>
       </c>
       <c r="Z2" s="1"/>
-      <c r="XFC2" s="0"/>
-      <c r="XFD2" s="0"/>
+      <c r="XFC2" s="1"/>
+      <c r="XFD2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -10287,7 +10283,7 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="2" sqref="J13 L13 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11375,7 +11371,7 @@
   <dimension ref="A1:XFD30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="2" sqref="J13 L13 A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13517,8 +13513,8 @@
   </sheetPr>
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13 L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14561,6 +14557,9 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>2200000</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>106</v>
       </c>
@@ -14582,56 +14581,63 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>4600</v>
+      </c>
       <c r="L19" s="3" t="n">
         <f aca="false">L18+L17</f>
         <v>424364.845714286</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J20" s="54" t="n">
+      <c r="B20" s="0" t="n">
+        <f aca="false">B18/B19</f>
+        <v>478.260869565217</v>
+      </c>
+      <c r="J20" s="3" t="n">
         <f aca="false">SUM(J3:J8)</f>
         <v>7280881.79664799</v>
       </c>
-      <c r="K20" s="54" t="n">
+      <c r="K20" s="3" t="n">
         <f aca="false">SUM(K3:K8)</f>
         <v>11297843.2080586</v>
       </c>
-      <c r="L20" s="54" t="n">
+      <c r="L20" s="3" t="n">
         <f aca="false">SUM(L3:L8)</f>
         <v>4791966.04904341</v>
       </c>
-      <c r="M20" s="54" t="n">
+      <c r="M20" s="3" t="n">
         <f aca="false">SUM(M3:M8)</f>
         <v>7842420.64395605</v>
       </c>
-      <c r="N20" s="54" t="n">
+      <c r="N20" s="3" t="n">
         <f aca="false">SUM(N3:N8)</f>
         <v>4949989.75919232</v>
       </c>
-      <c r="O20" s="54" t="n">
+      <c r="O20" s="3" t="n">
         <f aca="false">SUM(O3:O8)</f>
         <v>8213110.31135531</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J21" s="54" t="n">
+      <c r="J21" s="3" t="n">
         <f aca="false">J20*1.5</f>
         <v>10921322.694972</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54" t="n">
+      <c r="K21" s="3"/>
+      <c r="L21" s="3" t="n">
         <f aca="false">L20*1.5</f>
         <v>7187949.07356512</v>
       </c>
-      <c r="M21" s="54" t="n">
+      <c r="M21" s="3" t="n">
         <f aca="false">M20*1.5</f>
         <v>11763630.9659341</v>
       </c>
-      <c r="N21" s="54" t="n">
+      <c r="N21" s="3" t="n">
         <f aca="false">N20*1.5</f>
         <v>7424984.63878847</v>
       </c>
-      <c r="O21" s="54" t="n">
+      <c r="O21" s="3" t="n">
         <f aca="false">O20*1.5</f>
         <v>12319665.467033</v>
       </c>

</xml_diff>